<commit_message>
fucking around with flags
</commit_message>
<xml_diff>
--- a/plans/Pacific Federation Focus Tree.xlsx
+++ b/plans/Pacific Federation Focus Tree.xlsx
@@ -45,6 +45,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Frank Merriam (disjointed)</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -89,11 +113,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-"Suspend the Constitution" and "The Pacific Spirit" are available for both Charles Martin and Hiram Johnson</t>
+"Suspend the Constitution" and "The Pacific Spirit" are available for both Charles Martin and Hiram Johnson but nor Merriam</t>
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +137,55 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Frank Merriam (disjointed)</t>
+These only give cores, however they're permanent</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Requires the Western Federation focus</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Requires proclaiming the rival government</t>
         </r>
       </text>
     </comment>
@@ -141,12 +213,396 @@
         </r>
       </text>
     </comment>
+    <comment ref="O6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Nebraska and Kansas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Minnesota, Iowa and Missouri</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on all four Dakotas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Oklahoma and Northern Texas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Trans-Pecos and Southern Texas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Wisconsin, North Michigan and Illinois</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Michigan, Indiana and Ohio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Arkansas, Louisiana and Mississippi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Tennessee, Alabama and Georgia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Kentucky, the Virginias, and other states</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on all other states</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Coring Florida, Georgia, South Carolina and North Carolina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core on Maine and New England</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Only for Merriam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unavailable for Charles Martin</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Only for Charles Martin</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="190">
   <si>
     <t>Illyria  Parties</t>
   </si>
@@ -523,9 +979,6 @@
     <t>Deport Asian Immigrants</t>
   </si>
   <si>
-    <t>Suspend the Constitution</t>
-  </si>
-  <si>
     <t>The Pacific Spirit</t>
   </si>
   <si>
@@ -550,13 +1003,175 @@
     <t>Bureaucratic Ties</t>
   </si>
   <si>
-    <t>True American</t>
-  </si>
-  <si>
     <t>End Welfare</t>
   </si>
   <si>
     <t>Found the Pacific Secret Police</t>
+  </si>
+  <si>
+    <t>Tax Reforms</t>
+  </si>
+  <si>
+    <t>Finish Government Reforms</t>
+  </si>
+  <si>
+    <t>Help from Investors</t>
+  </si>
+  <si>
+    <t>Encourage Capitalism</t>
+  </si>
+  <si>
+    <t>Untouchable and Uncorrupted</t>
+  </si>
+  <si>
+    <t>Reject the Constitution</t>
+  </si>
+  <si>
+    <t>Independent Pacific State</t>
+  </si>
+  <si>
+    <t>Proclaim Rival Government</t>
+  </si>
+  <si>
+    <t>The Western Federation</t>
+  </si>
+  <si>
+    <t>The Constitution is Safe</t>
+  </si>
+  <si>
+    <t>Develop Underground Network</t>
+  </si>
+  <si>
+    <t>Incorporating Nevada</t>
+  </si>
+  <si>
+    <t>Incorporating Idaho</t>
+  </si>
+  <si>
+    <t>Conquest of Montana</t>
+  </si>
+  <si>
+    <t>Conquest of Arizona</t>
+  </si>
+  <si>
+    <t>Integrating Utah</t>
+  </si>
+  <si>
+    <t>Integrating Wyoming</t>
+  </si>
+  <si>
+    <t>Proclaim the Western Federation</t>
+  </si>
+  <si>
+    <t>Taking Over Colorado</t>
+  </si>
+  <si>
+    <t>Taking Over New Mexico</t>
+  </si>
+  <si>
+    <t>Victory Over Washington</t>
+  </si>
+  <si>
+    <t>Spread Influence to the East</t>
+  </si>
+  <si>
+    <t>The Dakotas</t>
+  </si>
+  <si>
+    <t>Midwest Expansion II</t>
+  </si>
+  <si>
+    <t>Midwest Expansion I</t>
+  </si>
+  <si>
+    <t>Southwest Expansion I</t>
+  </si>
+  <si>
+    <t>Southwest Expansion II</t>
+  </si>
+  <si>
+    <t>Midwest Dominance I</t>
+  </si>
+  <si>
+    <t>Midwest Dominance II</t>
+  </si>
+  <si>
+    <t>South Dominance I</t>
+  </si>
+  <si>
+    <t>South Dominance II</t>
+  </si>
+  <si>
+    <t>South Conquest</t>
+  </si>
+  <si>
+    <t>Atlantic Conquest II</t>
+  </si>
+  <si>
+    <t>Atlantic Conquest I</t>
+  </si>
+  <si>
+    <t>New England Conquest</t>
+  </si>
+  <si>
+    <t>Proclaim the Restoration of the United States</t>
+  </si>
+  <si>
+    <t>Sovereignity Secured</t>
+  </si>
+  <si>
+    <t>Seek International Recognition</t>
+  </si>
+  <si>
+    <t>Diplomatic Missions</t>
+  </si>
+  <si>
+    <t>Open Embassies</t>
+  </si>
+  <si>
+    <t>Diplomatic Outlook</t>
+  </si>
+  <si>
+    <t>Seek Japanese Backing</t>
+  </si>
+  <si>
+    <t>Seek Vesperian Backing</t>
+  </si>
+  <si>
+    <t>Seek Mexican Backing</t>
+  </si>
+  <si>
+    <t>Recognise Asian Immigrants</t>
+  </si>
+  <si>
+    <t>Vesperian-Pacific Economic Pact</t>
+  </si>
+  <si>
+    <t>Cascadian Bioregion</t>
+  </si>
+  <si>
+    <t>Seek Italian Backing</t>
+  </si>
+  <si>
+    <t>Alliance with Italy</t>
+  </si>
+  <si>
+    <t>Alliance with Japan</t>
+  </si>
+  <si>
+    <t>Alliance with Vesperia</t>
+  </si>
+  <si>
+    <t>Alliance with Mexico</t>
+  </si>
+  <si>
+    <t>Recognise Italian-Americans</t>
+  </si>
+  <si>
+    <t>Recognise the Hispanic</t>
+  </si>
+  <si>
+    <t>The Great Depression</t>
   </si>
 </sst>
 </file>
@@ -654,18 +1269,33 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -676,7 +1306,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -704,7 +1334,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1049,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1059,124 +1701,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="M1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="N1" s="23"/>
+      <c r="P1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q1" s="23"/>
+      <c r="V1" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="W1" s="23"/>
+      <c r="AC1" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD1" s="22"/>
     </row>
     <row r="2" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="J2" s="21" t="s">
+      <c r="C2" s="23"/>
+      <c r="F2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="J2" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="21"/>
+      <c r="K2" s="23"/>
+      <c r="M2" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="N2" s="22"/>
+      <c r="S2" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="T2" s="22"/>
     </row>
     <row r="3" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="J3" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="22"/>
+      <c r="M3" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="X3" s="22"/>
+    </row>
+    <row r="4" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="E3" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="F4" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="22"/>
+      <c r="K4" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" s="25"/>
+      <c r="M4" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P4" s="22"/>
+      <c r="R4" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="U4" s="22"/>
+      <c r="W4" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="X4" s="22"/>
+    </row>
+    <row r="5" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="E5" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="J5" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="22"/>
+      <c r="M5" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="N5" s="22"/>
+      <c r="P5" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q5" s="23"/>
+      <c r="V5" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="W5" s="23"/>
+    </row>
+    <row r="6" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="J3" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="21"/>
-    </row>
-    <row r="4" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="F4" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="I4" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="L4" s="21"/>
-    </row>
-    <row r="5" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="J5" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="K5" s="21"/>
-    </row>
-    <row r="6" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21" t="s">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21" t="s">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L6" s="21"/>
+      <c r="L6" s="22"/>
+      <c r="O6" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="X6" s="22"/>
     </row>
     <row r="7" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="21"/>
+      <c r="B7" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="22"/>
       <c r="D7" s="20"/>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="21"/>
+      <c r="G7" s="22"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="K7" s="21"/>
+      <c r="J7" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" s="22"/>
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
+      <c r="P7" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="W7" s="21"/>
       <c r="X7" s="20"/>
       <c r="Y7" s="20"/>
       <c r="Z7" s="20"/>
@@ -1191,8 +1953,10 @@
     <row r="8" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="21"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
@@ -1201,14 +1965,22 @@
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
+      <c r="P8" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="U8" s="21"/>
+      <c r="V8" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="W8" s="22"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
@@ -1221,24 +1993,32 @@
       <c r="AG8" s="20"/>
     </row>
     <row r="9" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="22"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="21"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="J9" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="K9" s="21"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
+      <c r="N9" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="O9" s="21"/>
+      <c r="S9" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="T9" s="22"/>
       <c r="V9" s="20"/>
       <c r="W9" s="20"/>
       <c r="X9" s="20"/>
@@ -1253,19 +2033,30 @@
       <c r="AG9" s="20"/>
     </row>
     <row r="10" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
+      <c r="A10" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
@@ -1285,18 +2076,22 @@
       <c r="AG10" s="20"/>
     </row>
     <row r="11" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="F11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="21"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
@@ -1317,18 +2112,28 @@
       <c r="AG11" s="20"/>
     </row>
     <row r="12" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="22"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="F12" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="21"/>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
+      <c r="J12" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="K12" s="21"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
+      <c r="N12" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="O12" s="21"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
@@ -1349,16 +2154,7 @@
       <c r="AG12" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
+  <mergeCells count="81">
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="B7:C7"/>
@@ -1371,10 +2167,75 @@
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="R4:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
two extra laws prototype
</commit_message>
<xml_diff>
--- a/plans/Pacific Federation Focus Tree.xlsx
+++ b/plans/Pacific Federation Focus Tree.xlsx
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
   <si>
     <t>Illyria  Parties</t>
   </si>
@@ -1172,6 +1172,42 @@
   </si>
   <si>
     <t>The Great Depression</t>
+  </si>
+  <si>
+    <t>Pacific Development Program</t>
+  </si>
+  <si>
+    <t>South Californian Civillian Sector</t>
+  </si>
+  <si>
+    <t>South Californian Military Sector</t>
+  </si>
+  <si>
+    <t>Oregon Civillian Sector</t>
+  </si>
+  <si>
+    <t>Oregon Military Sector</t>
+  </si>
+  <si>
+    <t>North Californian Civillian Sector</t>
+  </si>
+  <si>
+    <t>North Californian Military Sector</t>
+  </si>
+  <si>
+    <t>Pacific Railways</t>
+  </si>
+  <si>
+    <t>Expand State Highways</t>
+  </si>
+  <si>
+    <t>Industrial Boom</t>
+  </si>
+  <si>
+    <t>Expand Civillian Industry</t>
+  </si>
+  <si>
+    <t>Expand Military Industry</t>
   </si>
 </sst>
 </file>
@@ -1334,19 +1370,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1691,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" topLeftCell="U5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8:AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1701,262 +1737,300 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="M1" s="23" t="s">
+      <c r="G1" s="21"/>
+      <c r="M1" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="P1" s="23" t="s">
+      <c r="N1" s="24"/>
+      <c r="P1" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="V1" s="23" t="s">
+      <c r="Q1" s="24"/>
+      <c r="V1" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="W1" s="23"/>
-      <c r="AC1" s="22" t="s">
+      <c r="W1" s="24"/>
+      <c r="AC1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="AD1" s="22"/>
+      <c r="AD1" s="21"/>
     </row>
     <row r="2" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="F2" s="23" t="s">
+      <c r="C2" s="24"/>
+      <c r="F2" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="J2" s="23" t="s">
+      <c r="G2" s="24"/>
+      <c r="J2" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="M2" s="22" t="s">
+      <c r="K2" s="24"/>
+      <c r="M2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="S2" s="22" t="s">
+      <c r="N2" s="21"/>
+      <c r="S2" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="T2" s="22"/>
+      <c r="T2" s="21"/>
     </row>
     <row r="3" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="J3" s="22" t="s">
+      <c r="H3" s="21"/>
+      <c r="J3" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="M3" s="22" t="s">
+      <c r="K3" s="21"/>
+      <c r="M3" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22" t="s">
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22" t="s">
+      <c r="R3" s="21"/>
+      <c r="S3" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22" t="s">
+      <c r="T3" s="21"/>
+      <c r="U3" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22" t="s">
+      <c r="V3" s="21"/>
+      <c r="W3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="22"/>
+      <c r="X3" s="21"/>
     </row>
     <row r="4" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="F4" s="22" t="s">
+      <c r="D4" s="21"/>
+      <c r="F4" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="I4" s="22" t="s">
+      <c r="G4" s="21"/>
+      <c r="I4" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="24" t="s">
+      <c r="J4" s="21"/>
+      <c r="K4" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="22" t="s">
+      <c r="L4" s="23"/>
+      <c r="M4" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22" t="s">
+      <c r="N4" s="21"/>
+      <c r="O4" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="R4" s="22" t="s">
+      <c r="P4" s="21"/>
+      <c r="R4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22" t="s">
+      <c r="S4" s="21"/>
+      <c r="T4" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="U4" s="22"/>
-      <c r="W4" s="22" t="s">
+      <c r="U4" s="21"/>
+      <c r="W4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="X4" s="22"/>
+      <c r="X4" s="21"/>
+      <c r="AC4" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD4" s="21"/>
     </row>
     <row r="5" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="E5" s="22" t="s">
+      <c r="C5" s="21"/>
+      <c r="E5" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="J5" s="22" t="s">
+      <c r="H5" s="21"/>
+      <c r="J5" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="M5" s="22" t="s">
+      <c r="K5" s="21"/>
+      <c r="M5" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="P5" s="23" t="s">
+      <c r="N5" s="21"/>
+      <c r="P5" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="Q5" s="23"/>
-      <c r="V5" s="23" t="s">
+      <c r="Q5" s="24"/>
+      <c r="V5" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="W5" s="23"/>
+      <c r="W5" s="24"/>
+      <c r="Z5" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG5" s="21"/>
     </row>
     <row r="6" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="21"/>
+      <c r="G6" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22" t="s">
+      <c r="H6" s="21"/>
+      <c r="I6" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="O6" s="22" t="s">
+      <c r="L6" s="21"/>
+      <c r="O6" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22" t="s">
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22" t="s">
+      <c r="R6" s="21"/>
+      <c r="S6" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22" t="s">
+      <c r="T6" s="21"/>
+      <c r="U6" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22" t="s">
+      <c r="V6" s="21"/>
+      <c r="W6" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="X6" s="22"/>
+      <c r="X6" s="21"/>
+      <c r="Z6" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="AG6" s="21"/>
     </row>
     <row r="7" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="20"/>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="21"/>
       <c r="I7" s="20"/>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="K7" s="22"/>
+      <c r="K7" s="21"/>
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21" t="s">
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21" t="s">
+      <c r="S7" s="25"/>
+      <c r="T7" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21" t="s">
+      <c r="U7" s="25"/>
+      <c r="V7" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="W7" s="21"/>
+      <c r="W7" s="25"/>
       <c r="X7" s="20"/>
       <c r="Y7" s="20"/>
       <c r="Z7" s="20"/>
       <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="20"/>
-      <c r="AD7" s="20"/>
-      <c r="AE7" s="20"/>
-      <c r="AF7" s="20"/>
-      <c r="AG7" s="20"/>
+      <c r="AB7" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="AE7" s="25"/>
     </row>
     <row r="8" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
@@ -1965,60 +2039,62 @@
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21" t="s">
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21" t="s">
+      <c r="S8" s="25"/>
+      <c r="T8" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="U8" s="21"/>
-      <c r="V8" s="22" t="s">
+      <c r="U8" s="25"/>
+      <c r="V8" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="W8" s="22"/>
+      <c r="W8" s="21"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20"/>
+      <c r="AC8" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD8" s="25"/>
       <c r="AE8" s="20"/>
       <c r="AF8" s="20"/>
       <c r="AG8" s="20"/>
     </row>
     <row r="9" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="21"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="K9" s="21"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="S9" s="22" t="s">
+      <c r="O9" s="25"/>
+      <c r="S9" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="T9" s="22"/>
+      <c r="T9" s="21"/>
       <c r="V9" s="20"/>
       <c r="W9" s="20"/>
       <c r="X9" s="20"/>
@@ -2033,30 +2109,30 @@
       <c r="AG9" s="20"/>
     </row>
     <row r="10" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21" t="s">
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21" t="s">
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
@@ -2076,22 +2152,22 @@
       <c r="AG10" s="20"/>
     </row>
     <row r="11" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="20"/>
@@ -2112,28 +2188,28 @@
       <c r="AG11" s="20"/>
     </row>
     <row r="12" spans="1:33" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="G12" s="21"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="K12" s="21"/>
+      <c r="K12" s="25"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="O12" s="21"/>
+      <c r="O12" s="25"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
@@ -2154,40 +2230,51 @@
       <c r="AG12" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="93">
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="M2:N2"/>
@@ -2204,38 +2291,39 @@
     <mergeCell ref="T7:U7"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="S3:T3"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>